<commit_message>
added word document with project goal, variable description and analysis, description of implemented methods
</commit_message>
<xml_diff>
--- a/LinearOrderingProject/dane_do_wczytania.xlsx
+++ b/LinearOrderingProject/dane_do_wczytania.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Desktop\Statystyka\Python\StatisticalDataAnalysis\LinearOrderingProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kuba\Desktop\Python\Statystyka\StatisticalDataAnalysis\LinearOrderingProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{282CB285-58D8-4F95-B67B-DA98A48FE89C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{854DC9AB-52C8-4340-A081-DF9813208731}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{6A70AD75-653E-4EA5-84D2-BC63DA0A9DF3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6A70AD75-653E-4EA5-84D2-BC63DA0A9DF3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,18 +41,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
-    <t>zgony ogolem na tys urodzen zywych [liczba/tys urodzen zywych]</t>
-  </si>
-  <si>
-    <t>liczba ludnosci na lozko w szpitalach ogolnych [osoby/lozko]</t>
-  </si>
-  <si>
-    <t>absolwenci uczelni medycznych [osoba]</t>
-  </si>
-  <si>
-    <t>organizacje non profit ochrona zdrowia [%]</t>
-  </si>
-  <si>
     <t>MALOPOLSKIE</t>
   </si>
   <si>
@@ -101,19 +89,31 @@
     <t>MAZOWIECKIE</t>
   </si>
   <si>
-    <t>lekarze [liczba/tys ludnosci]</t>
-  </si>
-  <si>
-    <t>pielegniarki [liczba/tys ludnosci]</t>
-  </si>
-  <si>
-    <t>apteki [liczba/km2]</t>
-  </si>
-  <si>
-    <t>zespoly ratownictwa medycznego [liczba/tys ludnosci]</t>
-  </si>
-  <si>
     <t>wojewodztwo</t>
+  </si>
+  <si>
+    <t>lekarze</t>
+  </si>
+  <si>
+    <t>pielegniarki</t>
+  </si>
+  <si>
+    <t>apteki</t>
+  </si>
+  <si>
+    <t>zgony_ogolem</t>
+  </si>
+  <si>
+    <t>zespoly_ratownictwa</t>
+  </si>
+  <si>
+    <t>ludnosc_na_lozko</t>
+  </si>
+  <si>
+    <t>absolwenci</t>
+  </si>
+  <si>
+    <t>organizacje_non_profit_ochrona_zdrowia</t>
   </si>
 </sst>
 </file>
@@ -613,7 +613,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,36 +623,36 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
         <v>24</v>
-      </c>
-      <c r="B1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>4.1508641924923548</v>
@@ -682,7 +682,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>4.2255967275677282</v>
@@ -712,7 +712,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>2.7123562897644824</v>
@@ -742,7 +742,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>3.4285420410682192</v>
@@ -772,7 +772,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>3.9502551484224435</v>
@@ -802,7 +802,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>4.3696121805268939</v>
@@ -832,7 +832,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>2.8126251871218031</v>
@@ -862,7 +862,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>3.3954166088456277</v>
@@ -892,7 +892,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>4.1861510219482518</v>
@@ -922,7 +922,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>2.9853786280643049</v>
@@ -952,7 +952,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>5.015553560617132</v>
@@ -982,7 +982,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>3.5505898003687828</v>
@@ -1012,7 +1012,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>4.4679389687484665</v>
@@ -1042,7 +1042,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>3.1707679548211112</v>
@@ -1072,7 +1072,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>4.8480047357058291</v>
@@ -1102,7 +1102,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>5.0734745927198386</v>

</xml_diff>